<commit_message>
Add a web-services files and bug reports
</commit_message>
<xml_diff>
--- a/Check-list.xlsx
+++ b/Check-list.xlsx
@@ -4,23 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
     <sheet name="TCL1" sheetId="2" r:id="rId2"/>
     <sheet name="TCP1" sheetId="3" r:id="rId3"/>
-    <sheet name="TCP2" sheetId="4" r:id="rId4"/>
-    <sheet name="TCP3" sheetId="5" r:id="rId5"/>
-    <sheet name="TC4" sheetId="6" r:id="rId6"/>
-    <sheet name="TC5" sheetId="7" r:id="rId7"/>
+    <sheet name="TCP3" sheetId="4" r:id="rId4"/>
+    <sheet name="TCP5" sheetId="5" r:id="rId5"/>
+    <sheet name="TC7" sheetId="6" r:id="rId6"/>
+    <sheet name="TC9" sheetId="7" r:id="rId7"/>
+    <sheet name="bug #1" sheetId="8" r:id="rId8"/>
+    <sheet name="bug#2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="87">
   <si>
     <t>Проверка</t>
   </si>
@@ -41,12 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Log in</t>
-  </si>
-  <si>
-    <t>Запросы</t>
-  </si>
-  <si>
-    <t>Windows 10/64x, 1909</t>
   </si>
   <si>
     <t>languages</t>
@@ -112,12 +109,6 @@
     <t>TCP1</t>
   </si>
   <si>
-    <t>GET /genres</t>
-  </si>
-  <si>
-    <t>Code status is not 200 and status is not success</t>
-  </si>
-  <si>
     <t>Code status is 200 and status is success</t>
   </si>
   <si>
@@ -130,12 +121,6 @@
     <t>TCP2</t>
   </si>
   <si>
-    <t>GET /companies</t>
-  </si>
-  <si>
-    <t>GET /series</t>
-  </si>
-  <si>
     <t>companies with id=(-1),48</t>
   </si>
   <si>
@@ -181,20 +166,134 @@
     <t>GET /languages</t>
   </si>
   <si>
-    <t>GET /search</t>
-  </si>
-  <si>
     <t>1. Send request "https://api4.thetvdb.com/v4/languages"</t>
   </si>
   <si>
     <t>bug#2</t>
+  </si>
+  <si>
+    <t>GET /genres negative</t>
+  </si>
+  <si>
+    <t>GET /genres positive</t>
+  </si>
+  <si>
+    <t>TCP3</t>
+  </si>
+  <si>
+    <t>TCP4</t>
+  </si>
+  <si>
+    <t>GET /companies positive</t>
+  </si>
+  <si>
+    <t>GET /companies negative</t>
+  </si>
+  <si>
+    <t>TCP5</t>
+  </si>
+  <si>
+    <t>TCP6</t>
+  </si>
+  <si>
+    <t>GET /series positive</t>
+  </si>
+  <si>
+    <t>GET /series negative</t>
+  </si>
+  <si>
+    <t>TCP7</t>
+  </si>
+  <si>
+    <t>TCP8</t>
+  </si>
+  <si>
+    <t>GET /search positive</t>
+  </si>
+  <si>
+    <t>GET /search negative</t>
+  </si>
+  <si>
+    <t>Запросы GET</t>
+  </si>
+  <si>
+    <t>Windows 10 pro/64x, v.1909</t>
+  </si>
+  <si>
+    <t>Code status is NOT 200 and status is NOT success</t>
+  </si>
+  <si>
+    <t>Code status is NOT 200 and status is NOT success or failure</t>
+  </si>
+  <si>
+    <t>Defect ID</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Reporter</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Searches for invalid parameters</t>
+  </si>
+  <si>
+    <t>Data found</t>
+  </si>
+  <si>
+    <t>Kirill</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>1. Send request "https://api4.thetvdb.com/v4/language"</t>
+  </si>
+  <si>
+    <t>400 bad request</t>
+  </si>
+  <si>
+    <t>Status code is 200 and non-empty page found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad request when getting the page </t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Message about invalid parameters or status is failure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +344,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +372,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -376,37 +489,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -434,8 +545,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -737,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,96 +891,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="9"/>
+      <c r="B10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -852,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,69 +1022,74 @@
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="I1" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H3" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -940,7 +1101,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,75 +1114,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>33</v>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1033,7 +1198,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,75 +1207,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>33</v>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="8"/>
+      <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1122,7 +1291,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,75 +1303,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>33</v>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1214,7 +1387,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,79 +1396,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" location="'bug #1'!A1" display="bug#1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1305,7 +1485,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,69 +1494,234 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>33</v>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>54</v>
+      <c r="H2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="8"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" location="'bug#2'!A1" display="bug#2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>